<commit_message>
version finale du rapport
</commit_message>
<xml_diff>
--- a/src/Corolle.xlsx
+++ b/src/Corolle.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="37">
   <si>
     <t>Z1</t>
   </si>
@@ -70,12 +70,78 @@
   <si>
     <t>PI</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Z10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14:0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,8 +155,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,8 +260,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -441,11 +539,577 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -631,6 +1295,246 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -926,15 +1830,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC24"/>
+  <dimension ref="A1:AE58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AN56" sqref="AN56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="5" style="4"/>
+    <col min="1" max="19" width="5" style="4"/>
+    <col min="20" max="22" width="4.875" style="4" customWidth="1"/>
+    <col min="23" max="16384" width="5" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1458,8 +2364,8 @@
       <c r="M19" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="N19" s="53" t="s">
-        <v>6</v>
+      <c r="N19" s="139" t="s">
+        <v>16</v>
       </c>
       <c r="O19" s="52" t="s">
         <v>4</v>
@@ -1501,8 +2407,8 @@
       <c r="J20" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="K20" s="53" t="s">
-        <v>6</v>
+      <c r="K20" s="139" t="s">
+        <v>16</v>
       </c>
       <c r="L20" s="55" t="s">
         <v>7</v>
@@ -1613,8 +2519,8 @@
       <c r="N22" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="O22" s="53" t="s">
-        <v>6</v>
+      <c r="O22" s="139" t="s">
+        <v>16</v>
       </c>
       <c r="P22" s="46" t="s">
         <v>3</v>
@@ -1654,8 +2560,8 @@
       <c r="K23" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="L23" s="53" t="s">
-        <v>6</v>
+      <c r="L23" s="139" t="s">
+        <v>16</v>
       </c>
       <c r="M23" s="54" t="s">
         <v>9</v>
@@ -1714,9 +2620,766 @@
         <v>0</v>
       </c>
     </row>
+    <row r="26" spans="2:29" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:29" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="64"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="67"/>
+      <c r="J27" s="133" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" s="65"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="76"/>
+      <c r="N27" s="83"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="134" t="s">
+        <v>15</v>
+      </c>
+      <c r="S27" s="100"/>
+      <c r="T27" s="111"/>
+      <c r="U27" s="104"/>
+      <c r="V27" s="105"/>
+      <c r="W27" s="126"/>
+      <c r="X27" s="85"/>
+      <c r="Y27" s="111"/>
+      <c r="Z27" s="104"/>
+      <c r="AA27" s="105"/>
+      <c r="AB27" s="101"/>
+    </row>
+    <row r="28" spans="2:29" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="66"/>
+      <c r="C28" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="93"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="88"/>
+      <c r="G28" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="68"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="72"/>
+      <c r="M28" s="138"/>
+      <c r="N28" s="74"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="68"/>
+      <c r="S28" s="119"/>
+      <c r="T28" s="63"/>
+      <c r="U28" s="63"/>
+      <c r="V28" s="63"/>
+      <c r="W28" s="121"/>
+      <c r="X28" s="116"/>
+      <c r="Y28" s="63"/>
+      <c r="Z28" s="63"/>
+      <c r="AA28" s="63"/>
+      <c r="AB28" s="117"/>
+    </row>
+    <row r="29" spans="2:29" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="71"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="70"/>
+      <c r="J29" s="88"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="100"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="101"/>
+      <c r="O29" s="74"/>
+      <c r="P29" s="93"/>
+      <c r="S29" s="120"/>
+      <c r="T29" s="63"/>
+      <c r="U29" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="V29" s="68"/>
+      <c r="W29" s="132"/>
+      <c r="X29" s="131"/>
+      <c r="Y29" s="66"/>
+      <c r="Z29" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA29" s="63"/>
+      <c r="AB29" s="108"/>
+    </row>
+    <row r="30" spans="2:29" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="96"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="80"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="87"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="137"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="137"/>
+      <c r="P30" s="76"/>
+      <c r="S30" s="109"/>
+      <c r="T30" s="63"/>
+      <c r="U30" s="69"/>
+      <c r="V30" s="63"/>
+      <c r="W30" s="114"/>
+      <c r="X30" s="113"/>
+      <c r="Y30" s="63"/>
+      <c r="Z30" s="69"/>
+      <c r="AA30" s="63"/>
+      <c r="AB30" s="110"/>
+    </row>
+    <row r="31" spans="2:29" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="64"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="67"/>
+      <c r="J31" s="84"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="102"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="103"/>
+      <c r="O31" s="75"/>
+      <c r="P31" s="98"/>
+      <c r="S31" s="92"/>
+      <c r="T31" s="113"/>
+      <c r="U31" s="130"/>
+      <c r="V31" s="114"/>
+      <c r="W31" s="127"/>
+      <c r="X31" s="112"/>
+      <c r="Y31" s="113"/>
+      <c r="Z31" s="130"/>
+      <c r="AA31" s="114"/>
+      <c r="AB31" s="115"/>
+    </row>
+    <row r="32" spans="2:29" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="66"/>
+      <c r="C32" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="98"/>
+      <c r="E32" s="91"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="68"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="73"/>
+      <c r="M32" s="57"/>
+      <c r="N32" s="75"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="68"/>
+      <c r="S32" s="123"/>
+      <c r="T32" s="116"/>
+      <c r="U32" s="129"/>
+      <c r="V32" s="121"/>
+      <c r="W32" s="124"/>
+      <c r="X32" s="118"/>
+      <c r="Y32" s="116"/>
+      <c r="Z32" s="129"/>
+      <c r="AA32" s="121"/>
+      <c r="AB32" s="82"/>
+    </row>
+    <row r="33" spans="2:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="71"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="95"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="70"/>
+      <c r="J33" s="136" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="69"/>
+      <c r="L33" s="94"/>
+      <c r="M33" s="76"/>
+      <c r="N33" s="89"/>
+      <c r="O33" s="69"/>
+      <c r="P33" s="135" t="s">
+        <v>15</v>
+      </c>
+      <c r="S33" s="119"/>
+      <c r="T33" s="63"/>
+      <c r="U33" s="65"/>
+      <c r="V33" s="63"/>
+      <c r="W33" s="121"/>
+      <c r="X33" s="116"/>
+      <c r="Y33" s="63"/>
+      <c r="Z33" s="65"/>
+      <c r="AA33" s="63"/>
+      <c r="AB33" s="117"/>
+    </row>
+    <row r="34" spans="2:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S34" s="120"/>
+      <c r="T34" s="63"/>
+      <c r="U34" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="V34" s="68"/>
+      <c r="W34" s="132"/>
+      <c r="X34" s="128"/>
+      <c r="Y34" s="66"/>
+      <c r="Z34" s="99" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA34" s="63"/>
+      <c r="AB34" s="108"/>
+    </row>
+    <row r="35" spans="2:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S35" s="109"/>
+      <c r="T35" s="63"/>
+      <c r="U35" s="63"/>
+      <c r="V35" s="63"/>
+      <c r="W35" s="114"/>
+      <c r="X35" s="113"/>
+      <c r="Y35" s="63"/>
+      <c r="Z35" s="63"/>
+      <c r="AA35" s="63"/>
+      <c r="AB35" s="110"/>
+    </row>
+    <row r="36" spans="2:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S36" s="102"/>
+      <c r="T36" s="122"/>
+      <c r="U36" s="107"/>
+      <c r="V36" s="106"/>
+      <c r="W36" s="125"/>
+      <c r="X36" s="81"/>
+      <c r="Y36" s="122"/>
+      <c r="Z36" s="107"/>
+      <c r="AA36" s="106"/>
+      <c r="AB36" s="103"/>
+    </row>
+    <row r="37" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+    </row>
+    <row r="38" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+    </row>
+    <row r="39" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+    </row>
+    <row r="40" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+    </row>
+    <row r="41" spans="2:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+    </row>
+    <row r="42" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="5">
+        <v>4</v>
+      </c>
+      <c r="C42" s="6">
+        <v>20</v>
+      </c>
+      <c r="D42" s="6">
+        <v>20</v>
+      </c>
+      <c r="E42" s="6">
+        <v>20</v>
+      </c>
+      <c r="F42" s="6">
+        <v>20</v>
+      </c>
+      <c r="G42" s="6">
+        <v>20</v>
+      </c>
+      <c r="H42" s="7">
+        <v>4</v>
+      </c>
+      <c r="I42"/>
+      <c r="J42" s="5">
+        <v>1</v>
+      </c>
+      <c r="K42" s="6">
+        <v>7</v>
+      </c>
+      <c r="L42" s="6">
+        <v>20</v>
+      </c>
+      <c r="M42" s="6">
+        <v>20</v>
+      </c>
+      <c r="N42" s="6">
+        <v>20</v>
+      </c>
+      <c r="O42" s="6">
+        <v>20</v>
+      </c>
+      <c r="P42" s="7">
+        <v>3</v>
+      </c>
+      <c r="U42" s="141" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y42" s="141" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="8">
+        <v>20</v>
+      </c>
+      <c r="C43" s="3">
+        <v>100</v>
+      </c>
+      <c r="D43" s="3">
+        <v>100</v>
+      </c>
+      <c r="E43" s="3">
+        <v>100</v>
+      </c>
+      <c r="F43" s="3">
+        <v>100</v>
+      </c>
+      <c r="G43" s="3">
+        <v>100</v>
+      </c>
+      <c r="H43" s="9">
+        <v>20</v>
+      </c>
+      <c r="I43"/>
+      <c r="J43" s="8">
+        <v>7</v>
+      </c>
+      <c r="K43" s="63">
+        <v>58</v>
+      </c>
+      <c r="L43" s="3">
+        <v>100</v>
+      </c>
+      <c r="M43" s="3">
+        <v>100</v>
+      </c>
+      <c r="N43" s="3">
+        <v>100</v>
+      </c>
+      <c r="O43" s="3">
+        <v>100</v>
+      </c>
+      <c r="P43" s="9">
+        <v>20</v>
+      </c>
+      <c r="T43" s="141" t="s">
+        <v>13</v>
+      </c>
+      <c r="U43" s="141" t="s">
+        <v>14</v>
+      </c>
+      <c r="V43" s="141" t="s">
+        <v>14</v>
+      </c>
+      <c r="X43" s="141" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y43" s="141" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z43" s="141" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="8">
+        <v>20</v>
+      </c>
+      <c r="C44" s="63">
+        <v>100</v>
+      </c>
+      <c r="D44" s="140">
+        <v>100</v>
+      </c>
+      <c r="E44" s="3">
+        <v>100</v>
+      </c>
+      <c r="F44" s="3">
+        <v>100</v>
+      </c>
+      <c r="G44" s="3">
+        <v>100</v>
+      </c>
+      <c r="H44" s="9">
+        <v>20</v>
+      </c>
+      <c r="I44"/>
+      <c r="J44" s="8">
+        <v>20</v>
+      </c>
+      <c r="K44" s="63">
+        <v>100</v>
+      </c>
+      <c r="L44" s="3">
+        <v>100</v>
+      </c>
+      <c r="M44" s="3">
+        <v>100</v>
+      </c>
+      <c r="N44" s="3">
+        <v>100</v>
+      </c>
+      <c r="O44" s="3">
+        <v>100</v>
+      </c>
+      <c r="P44" s="9">
+        <v>20</v>
+      </c>
+      <c r="U44" s="141" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y44" s="141" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="8">
+        <v>20</v>
+      </c>
+      <c r="C45" s="3">
+        <v>100</v>
+      </c>
+      <c r="D45" s="3">
+        <v>100</v>
+      </c>
+      <c r="E45" s="3">
+        <v>100</v>
+      </c>
+      <c r="F45" s="3">
+        <v>100</v>
+      </c>
+      <c r="G45" s="3">
+        <v>100</v>
+      </c>
+      <c r="H45" s="9">
+        <v>20</v>
+      </c>
+      <c r="J45" s="8">
+        <v>20</v>
+      </c>
+      <c r="K45" s="3">
+        <v>100</v>
+      </c>
+      <c r="L45" s="3">
+        <v>100</v>
+      </c>
+      <c r="M45" s="3">
+        <v>100</v>
+      </c>
+      <c r="N45" s="3">
+        <v>100</v>
+      </c>
+      <c r="O45" s="3">
+        <v>100</v>
+      </c>
+      <c r="P45" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="8">
+        <v>20</v>
+      </c>
+      <c r="C46" s="3">
+        <v>100</v>
+      </c>
+      <c r="D46" s="3">
+        <v>100</v>
+      </c>
+      <c r="E46" s="3">
+        <v>100</v>
+      </c>
+      <c r="F46" s="3">
+        <v>100</v>
+      </c>
+      <c r="G46" s="3">
+        <v>100</v>
+      </c>
+      <c r="H46" s="9">
+        <v>20</v>
+      </c>
+      <c r="J46" s="8">
+        <v>20</v>
+      </c>
+      <c r="K46" s="3">
+        <v>100</v>
+      </c>
+      <c r="L46" s="3">
+        <v>100</v>
+      </c>
+      <c r="M46" s="3">
+        <v>100</v>
+      </c>
+      <c r="N46" s="3">
+        <v>100</v>
+      </c>
+      <c r="O46" s="3">
+        <v>100</v>
+      </c>
+      <c r="P46" s="9">
+        <v>20</v>
+      </c>
+      <c r="U46" s="141" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y46" s="141" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="8">
+        <v>20</v>
+      </c>
+      <c r="C47" s="3">
+        <v>100</v>
+      </c>
+      <c r="D47" s="3">
+        <v>100</v>
+      </c>
+      <c r="E47" s="3">
+        <v>100</v>
+      </c>
+      <c r="F47" s="3">
+        <v>100</v>
+      </c>
+      <c r="G47" s="3">
+        <v>100</v>
+      </c>
+      <c r="H47" s="9">
+        <v>20</v>
+      </c>
+      <c r="J47" s="8">
+        <v>20</v>
+      </c>
+      <c r="K47" s="3">
+        <v>100</v>
+      </c>
+      <c r="L47" s="3">
+        <v>100</v>
+      </c>
+      <c r="M47" s="3">
+        <v>100</v>
+      </c>
+      <c r="N47" s="3">
+        <v>100</v>
+      </c>
+      <c r="O47" s="3">
+        <v>100</v>
+      </c>
+      <c r="P47" s="9">
+        <v>20</v>
+      </c>
+      <c r="T47" s="141" t="s">
+        <v>13</v>
+      </c>
+      <c r="U47" s="141" t="s">
+        <v>14</v>
+      </c>
+      <c r="V47" s="141" t="s">
+        <v>14</v>
+      </c>
+      <c r="X47" s="141" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y47" s="141" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z47" s="141" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="2:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="10">
+        <v>4</v>
+      </c>
+      <c r="C48" s="11">
+        <v>20</v>
+      </c>
+      <c r="D48" s="11">
+        <v>20</v>
+      </c>
+      <c r="E48" s="11">
+        <v>20</v>
+      </c>
+      <c r="F48" s="11">
+        <v>20</v>
+      </c>
+      <c r="G48" s="11">
+        <v>20</v>
+      </c>
+      <c r="H48" s="12">
+        <v>4</v>
+      </c>
+      <c r="J48" s="10">
+        <v>3</v>
+      </c>
+      <c r="K48" s="11">
+        <v>20</v>
+      </c>
+      <c r="L48" s="11">
+        <v>20</v>
+      </c>
+      <c r="M48" s="11">
+        <v>20</v>
+      </c>
+      <c r="N48" s="11">
+        <v>20</v>
+      </c>
+      <c r="O48" s="11">
+        <v>20</v>
+      </c>
+      <c r="P48" s="12">
+        <v>3</v>
+      </c>
+      <c r="U48" s="141" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y48" s="141" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="20:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U52" s="142" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y52" s="141" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD52" s="141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="20:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T53" s="142" t="s">
+        <v>20</v>
+      </c>
+      <c r="U53" s="142" t="s">
+        <v>18</v>
+      </c>
+      <c r="V53" s="142" t="s">
+        <v>19</v>
+      </c>
+      <c r="X53" s="141" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y53" s="141" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z53" s="141" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC53" s="141">
+        <v>3</v>
+      </c>
+      <c r="AD53" s="141">
+        <v>0</v>
+      </c>
+      <c r="AE53" s="141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="20:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U54" s="142" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y54" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD54" s="141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="20:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U56" s="141" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y56" s="141" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="20:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T57" s="141" t="s">
+        <v>35</v>
+      </c>
+      <c r="U57" s="141" t="s">
+        <v>33</v>
+      </c>
+      <c r="V57" s="141" t="s">
+        <v>36</v>
+      </c>
+      <c r="X57" s="141" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y57" s="141" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z57" s="141" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="20:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U58" s="141" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y58" s="141" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B11:H12 I16 B8:F9 G14:G15 B13:F14 B10:G10">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="175">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1724,7 +3387,7 @@
         <color theme="4" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="32">
+    <cfRule type="colorScale" priority="176">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1732,15 +3395,15 @@
         <color rgb="FF00B0F0"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="177">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="178">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1752,7 +3415,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="171">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1760,7 +3423,7 @@
         <color theme="4" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="172">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1768,15 +3431,15 @@
         <color rgb="FF00B0F0"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="173">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1788,7 +3451,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:M8 L7 L9">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="183">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1796,7 +3459,7 @@
         <color theme="4" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="184">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1804,15 +3467,15 @@
         <color rgb="FF00B0F0"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="41">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="185">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="186">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1824,7 +3487,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12:O14">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="163">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1832,7 +3495,7 @@
         <color theme="4" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="164">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1840,15 +3503,15 @@
         <color rgb="FF00B0F0"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="165">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="166">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1860,7 +3523,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="159">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1868,7 +3531,7 @@
         <color theme="4" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="160">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1876,15 +3539,15 @@
         <color rgb="FF00B0F0"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="161">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="162">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1896,7 +3559,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P13">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="155">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1904,7 +3567,7 @@
         <color theme="4" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="156">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1912,15 +3575,15 @@
         <color rgb="FF00B0F0"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="157">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="158">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1932,7 +3595,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="151">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1940,7 +3603,7 @@
         <color theme="4" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="152">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1948,15 +3611,15 @@
         <color rgb="FF00B0F0"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="153">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="154">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1968,7 +3631,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="147">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1976,7 +3639,7 @@
         <color theme="4" tint="0.79998168889431442"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="148">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1984,15 +3647,15 @@
         <color rgb="FF00B0F0"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="149">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="150">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2004,7 +3667,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:Z10">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="146">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2014,8 +3677,944 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:H24">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Z1">
+    <cfRule type="containsText" dxfId="0" priority="145" operator="containsText" text="Z1">
       <formula>NOT(ISERROR(SEARCH("Z1",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T43:V43 U42 U44">
+    <cfRule type="colorScale" priority="141">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="142">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="143">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="144">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y42 Y44 X43:Z43">
+    <cfRule type="colorScale" priority="137">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="138">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="139">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="140">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y47">
+    <cfRule type="colorScale" priority="133">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="134">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="135">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="136">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T47:V47 U46">
+    <cfRule type="colorScale" priority="129">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="130">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="131">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="132">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z47">
+    <cfRule type="colorScale" priority="125">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="126">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="127">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="128">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y48">
+    <cfRule type="colorScale" priority="121">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="122">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="123">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="124">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y46">
+    <cfRule type="colorScale" priority="117">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="118">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="119">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="120">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X47">
+    <cfRule type="colorScale" priority="113">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="114">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="115">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="116">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U48">
+    <cfRule type="colorScale" priority="109">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="110">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="111">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="112">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T53:V53 U52 U54">
+    <cfRule type="colorScale" priority="105">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="106">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="107">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="108">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y52 Y54 X53:Z53">
+    <cfRule type="colorScale" priority="101">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="102">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="103">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="104">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z57">
+    <cfRule type="colorScale" priority="89">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="90">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="91">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="92">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y58">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X57">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y56">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="63">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y57">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U57">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U56">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V57">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U58">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T57">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD53">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE53">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD54">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD52">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC53">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <color theme="4" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF0070C0"/>
+        <color rgb="FF00B0F0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>